<commit_message>
fixing bug import spkl
</commit_message>
<xml_diff>
--- a/public/documents/template-spkl-rev.xlsx
+++ b/public/documents/template-spkl-rev.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{41E5EE2B-CF30-E441-A2FA-79B2041018EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="6360" yWindow="2200" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,65 +25,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NIK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipe Libur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EN-0</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>NIK</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Tipe Libur</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Lembur</t>
+  </si>
+  <si>
+    <t>Masuk</t>
+  </si>
+  <si>
+    <t>Input NIK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -93,7 +84,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
@@ -101,7 +92,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
@@ -124,109 +115,83 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF808080"/>
       </left>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -285,60 +250,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -370,7 +351,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -394,7 +375,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -454,46 +435,45 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.17"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" customWidth="1"/>
+    <col min="12" max="12" width="24.1640625" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" customWidth="1"/>
+    <col min="19" max="19" width="10.5" customWidth="1"/>
+    <col min="20" max="20" width="11.5" customWidth="1"/>
+    <col min="21" max="21" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,33 +496,37 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="10">
+        <v>45647</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5">
+        <v>3</v>
+      </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -551,7 +535,7 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -560,7 +544,7 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -570,7 +554,7 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -579,7 +563,7 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -588,7 +572,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="8"/>
@@ -598,28 +582,23 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C10" s="9"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D13" s="9"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D14" s="9"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D15" s="9"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D16" s="9"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>